<commit_message>
update minors. especially for db sw hw contents
</commit_message>
<xml_diff>
--- a/tabs/ZDATA__link_for_DBSW.xlsx
+++ b/tabs/ZDATA__link_for_DBSW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e64a25058d50c5c4/OneD-2025/6_homepage_byungkiryu/byungkiryu/tabs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="337" documentId="13_ncr:1_{17D0EB6A-8C48-4958-B4B1-97F25152412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EE2D076-90BF-477C-B659-53AD1FC39F6D}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="13_ncr:1_{17D0EB6A-8C48-4958-B4B1-97F25152412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0482D8DB-41B6-4802-A9D9-6FAACAC00982}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{6D651AE5-37C2-4486-97AE-FE18438EF94C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>name</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -71,9 +71,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Thermoelectric Power Generation Web Simulator Lite ver.0.53a</t>
-  </si>
-  <si>
     <t>TESimulator</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -92,22 +89,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Database of solution, segregation, binding, and doping energies of alloying elements for the design of high-performance Cu-Ni-Si alloys.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>A database of calculated solid solution, segregation, and binding characteristics of additive elements in lithium alloys for the design of high-strength, long-life anode materials in Li-S batteries.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Cu-Ni-Si Alloy Design DB (v0.1)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Thermoelectric simulator for power TGM, standalone, multistage, 1D</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>https://jaywan-chung.github.io/ml-tep-BiTe/</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -132,45 +117,65 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Machine Learning Model Predicting Thermoelectric Properties of BiTe-based materials ver.0.2a</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning Model Predicting Thermoelectric Properties of PbTe-based materials ver.0.1a</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning Model Predicting Strength and Conductivity of Copper alloys (POONGSAN data) ver.0.5b</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>webpage</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>DB</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>simulator</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ML</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>contenttype</t>
   </si>
   <si>
-    <t>Ultra-high quality thermoelectric material property database</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>https://cunisi-v01.streamlit.app/</t>
   </si>
   <si>
     <t>Alloy Design DB (v0.33)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning Model Predicting Thermoelectric Properties of BiTe-based materials ver.0.2a. Developed by Dr. Jaywan Chung. Engined by LaNN.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning Model Predicting Thermoelectric Properties of PbTe-based materials ver.0.1a. Developed by Dr. Jaywan Chung. Engined by LaNN.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning Model Predicting Strength and Conductivity of Copper alloys (POONGSAN data) ver.0.5b. Developed by Dr. Jaywan Chung. Engined by LaNN.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thermoelectric simulator for power TGM, standalone, multistage, 1D. Designed and devloped by Drs. Jaywan Chung and Byungki Ryu.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thermoelectric Power Generation Web Simulator Lite ver.0.53a. Developed by Dr. Jaywan Chung. Designed by Dr. Byungki Ryu.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alloy Design DB (v0.33). Data from KIMS. Designed and developed by Dr. Byungki Ryu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database of solution, segregation, binding, and doping energies of alloying elements for the design of high-performance Cu-Ni-Si alloys. Data from KIMS. Designed and developed by Dr. Byungki Ryu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>A database of calculated solid solution, segregation, and binding characteristics of additive elements in lithium alloys for the design of high-strength, long-life anode materials in Li-S batteries. Data from KIMS. Designed and developed by Dr. Byungki Ryu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ultra-high quality thermoelectric material property database. Developed by Dr. Byungki Ryu.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -833,7 +838,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -848,9 +853,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -991,19 +993,19 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <top style="thin">
           <color indexed="64"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1019,8 +1021,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}" name="표1" displayName="표1" ref="A1:D11" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}" name="표1" displayName="표1" ref="A1:D11" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:D11" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{96862A6D-D2E1-4EB2-BEFE-53F68ABEDF9F}" name="contenttype" dataDxfId="3"/>
@@ -1352,7 +1358,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -1364,146 +1370,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A2" s="6" t="s">
-        <v>29</v>
+    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A3" s="6" t="s">
-        <v>29</v>
+      <c r="A3" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
-      <c r="A4" s="6" t="s">
-        <v>29</v>
+    <row r="4" spans="1:4" ht="39.4" x14ac:dyDescent="0.6">
+      <c r="A4" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39.4" x14ac:dyDescent="0.6">
-      <c r="A5" s="6" t="s">
-        <v>29</v>
+      <c r="A5" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="A6" s="6" t="s">
-        <v>31</v>
+      <c r="A6" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="A7" s="6" t="s">
-        <v>31</v>
+      <c r="A7" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A11" s="6" t="s">
-        <v>28</v>
+      <c r="A11" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -1511,7 +1517,7 @@
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: small content, favicon
</commit_message>
<xml_diff>
--- a/tabs/ZDATA__link_for_DBSW.xlsx
+++ b/tabs/ZDATA__link_for_DBSW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e64a25058d50c5c4/OneD-2025/6_homepage_byungkiryu/byungkiryu/tabs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="359" documentId="13_ncr:1_{17D0EB6A-8C48-4958-B4B1-97F25152412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0482D8DB-41B6-4802-A9D9-6FAACAC00982}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="13_ncr:1_{17D0EB6A-8C48-4958-B4B1-97F25152412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2C55A8-A9B9-435B-B2E7-88E0A24F3BCE}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{6D651AE5-37C2-4486-97AE-FE18438EF94C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>name</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Dr. Byungki Ryu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>https://tematdbv114.streamlit.app/</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -121,10 +117,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>simulator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>contenttype</t>
   </si>
   <si>
@@ -176,6 +168,38 @@
   </si>
   <si>
     <t>Ultra-high quality thermoelectric material property database. Developed by Dr. Byungki Ryu.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main Link Hub</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main Link Hub github page - research, data, machine learning, simulators, and webpages.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://byungkiryu.github.io/link-home/</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr. Byungki Ryu's Legacy webpage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BR @ TES</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Byungki Ryu's research webpage for Thermoelectric Science Team at KERI</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://byungkiryu.streamlit.app/</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simulator</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -183,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +384,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -542,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -709,6 +741,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -838,7 +894,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -857,14 +913,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1026,8 +1100,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}" name="표1" displayName="표1" ref="A1:D11" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A1:D11" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}" name="표1" displayName="표1" ref="A1:D13" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:D13" xr:uid="{C361BD9B-6FA8-407A-AC48-AF447BAA9979}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{96862A6D-D2E1-4EB2-BEFE-53F68ABEDF9F}" name="contenttype" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{BB6212E7-76EA-4223-A6DC-497808E11B24}" name="name" dataDxfId="2"/>
@@ -1355,175 +1429,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5398742-1EB9-4AF8-BAE3-0DC7005D8EE1}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="16.0625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="61.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="73.5625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
+      <c r="A3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
+      <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
+      <c r="A5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="39.4" x14ac:dyDescent="0.6">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.4" x14ac:dyDescent="0.6">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="39.4" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
+    <row r="11" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="39.4" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="A6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="A7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="A13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26.25" x14ac:dyDescent="0.6">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
+      <c r="B13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D12">
+    <sortCondition ref="A5:A12"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>